<commit_message>
Created preliminary unique stack report
</commit_message>
<xml_diff>
--- a/Triage/Triage.Mortician.Analyzers/template.xlsx
+++ b/Triage/Triage.Mortician.Analyzers/template.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Object Counts" sheetId="2" r:id="rId1"/>
     <sheet name="Object Sizes" sheetId="3" r:id="rId2"/>
+    <sheet name="Unique Stacks" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Object Counts'!$A$1:$F$2946</definedName>
@@ -254,11 +255,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="230881152"/>
-        <c:axId val="230882688"/>
+        <c:axId val="222497024"/>
+        <c:axId val="222502912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="230881152"/>
+        <c:axId val="222497024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -268,7 +269,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230882688"/>
+        <c:crossAx val="222502912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -276,7 +277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="230882688"/>
+        <c:axId val="222502912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -287,14 +288,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230881152"/>
+        <c:crossAx val="222497024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -476,11 +476,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="231065472"/>
-        <c:axId val="231067008"/>
+        <c:axId val="222546176"/>
+        <c:axId val="222957568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="231065472"/>
+        <c:axId val="222546176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="231067008"/>
+        <c:crossAx val="222957568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="231067008"/>
+        <c:axId val="222957568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,14 +509,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="231065472"/>
+        <c:crossAx val="222546176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -890,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2946"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -36308,4 +36307,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added second chart view for objects
</commit_message>
<xml_diff>
--- a/Triage/Triage.Mortician.Analyzers/template.xlsx
+++ b/Triage/Triage.Mortician.Analyzers/template.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Object Counts" sheetId="2" r:id="rId1"/>
-    <sheet name="Object Sizes" sheetId="3" r:id="rId2"/>
+    <sheet name="Object Sizes" sheetId="5" r:id="rId2"/>
     <sheet name="Unique Stacks" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -255,11 +255,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="222497024"/>
-        <c:axId val="222502912"/>
+        <c:axId val="222107904"/>
+        <c:axId val="222113792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="222497024"/>
+        <c:axId val="222107904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,7 +269,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222502912"/>
+        <c:crossAx val="222113792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -277,7 +277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222502912"/>
+        <c:axId val="222113792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -288,13 +288,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222497024"/>
+        <c:crossAx val="222107904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -310,6 +311,227 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Counts'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gen0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Counts'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Counts'!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Counts'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gen1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Counts'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Counts'!$C$2:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Counts'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gen2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Counts'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Counts'!$D$2:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Counts'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LOH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Counts'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Counts'!$E$2:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="222144384"/>
+        <c:axId val="222145920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="222144384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="222145920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="222145920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="222144384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -476,11 +698,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="222546176"/>
-        <c:axId val="222957568"/>
+        <c:axId val="222288128"/>
+        <c:axId val="222437376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="222546176"/>
+        <c:axId val="222288128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222957568"/>
+        <c:crossAx val="222437376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222957568"/>
+        <c:axId val="222437376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,13 +731,235 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222546176"/>
+        <c:crossAx val="222288128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Sizes'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gen0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Sizes'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Sizes'!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Sizes'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gen1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Sizes'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Sizes'!$C$2:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Sizes'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gen2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Sizes'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Sizes'!$D$2:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Object Sizes'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LOH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Object Sizes'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Object Sizes'!$E$2:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="222478336"/>
+        <c:axId val="222479872"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="222478336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="222479872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="222479872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="222478336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -562,6 +1006,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -594,6 +1070,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -889,7 +1397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2946"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -36313,7 +36821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added Stack Frame excel tab This tab shows the unique stack frames and how many times they appear in the stack trace
</commit_message>
<xml_diff>
--- a/Triage/Triage.Mortician.Analyzers/template.xlsx
+++ b/Triage/Triage.Mortician.Analyzers/template.xlsx
@@ -4,23 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Object Counts" sheetId="2" r:id="rId1"/>
     <sheet name="Object Sizes" sheetId="5" r:id="rId2"/>
     <sheet name="Unique Stacks" sheetId="4" r:id="rId3"/>
+    <sheet name="Stack Frames" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Object Counts'!$A$1:$F$2946</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Object Sizes'!$A$1:$F$2946</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Stack Frames'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -38,6 +40,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Stack Frame</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -78,7 +89,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -255,11 +277,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="222107904"/>
-        <c:axId val="222113792"/>
+        <c:axId val="162732288"/>
+        <c:axId val="162742272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="222107904"/>
+        <c:axId val="162732288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,7 +291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222113792"/>
+        <c:crossAx val="162742272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -277,7 +299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222113792"/>
+        <c:axId val="162742272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -288,7 +310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222107904"/>
+        <c:crossAx val="162732288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -476,11 +498,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="222144384"/>
-        <c:axId val="222145920"/>
+        <c:axId val="162764672"/>
+        <c:axId val="162766208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="222144384"/>
+        <c:axId val="162764672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222145920"/>
+        <c:crossAx val="162766208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222145920"/>
+        <c:axId val="162766208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,14 +531,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222144384"/>
+        <c:crossAx val="162764672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -698,11 +719,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="222288128"/>
-        <c:axId val="222437376"/>
+        <c:axId val="162895744"/>
+        <c:axId val="162897280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="222288128"/>
+        <c:axId val="162895744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222437376"/>
+        <c:crossAx val="162897280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -720,7 +741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222437376"/>
+        <c:axId val="162897280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,7 +752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222288128"/>
+        <c:crossAx val="162895744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -919,11 +940,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="222478336"/>
-        <c:axId val="222479872"/>
+        <c:axId val="163325440"/>
+        <c:axId val="163326976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="222478336"/>
+        <c:axId val="163325440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +954,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222479872"/>
+        <c:crossAx val="163326976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -941,7 +962,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222479872"/>
+        <c:axId val="163326976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,14 +973,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222478336"/>
+        <c:crossAx val="163325440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1397,7 +1417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2946"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -36824,7 +36844,41 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the excel template Added Stack Frame summary
</commit_message>
<xml_diff>
--- a/Triage/Triage.Mortician.Analyzers/template.xlsx
+++ b/Triage/Triage.Mortician.Analyzers/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +91,24 @@
   <si>
     <t>Mortician Report</t>
   </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Std Deviation</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Avg Deviation</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
 </sst>
 </file>
 
@@ -99,11 +117,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -141,42 +166,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,11 +384,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="252382592"/>
-        <c:axId val="252400768"/>
+        <c:axId val="210880768"/>
+        <c:axId val="211222528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="252382592"/>
+        <c:axId val="210880768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252400768"/>
+        <c:crossAx val="211222528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -380,7 +406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252400768"/>
+        <c:axId val="211222528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,7 +417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252382592"/>
+        <c:crossAx val="210880768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -579,11 +605,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="252419072"/>
-        <c:axId val="252437248"/>
+        <c:axId val="210673024"/>
+        <c:axId val="210699392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="252419072"/>
+        <c:axId val="210673024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,7 +619,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252437248"/>
+        <c:crossAx val="210699392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -601,7 +627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252437248"/>
+        <c:axId val="210699392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,14 +638,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252419072"/>
+        <c:crossAx val="210673024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -801,11 +826,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="252599296"/>
-        <c:axId val="252605184"/>
+        <c:axId val="210765312"/>
+        <c:axId val="210766848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="252599296"/>
+        <c:axId val="210765312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252605184"/>
+        <c:crossAx val="210766848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -823,7 +848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252605184"/>
+        <c:axId val="210766848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,7 +859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252599296"/>
+        <c:crossAx val="210765312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1022,11 +1047,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="252719488"/>
-        <c:axId val="252721024"/>
+        <c:axId val="210973440"/>
+        <c:axId val="210974976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="252719488"/>
+        <c:axId val="210973440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252721024"/>
+        <c:crossAx val="210974976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1044,7 +1069,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252721024"/>
+        <c:axId val="210974976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1080,129 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252719488"/>
+        <c:crossAx val="210973440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stack Frames'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stack Frames'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stack Frames'!$C$2:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="226637696"/>
+        <c:axId val="226660352"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="226637696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="226660352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="226660352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="226637696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1205,6 +1352,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1498,11 +1680,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1514,91 +1694,86 @@
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="B1" s="7">
+        <f>SummaryData!B1</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="7">
-        <f>SummaryData!B1</f>
+        <v>9</v>
+      </c>
+      <c r="B2" s="9">
+        <f>SummaryData!B2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9">
-        <f>SummaryData!B2</f>
+        <f>SummaryData!B3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="9">
-        <f>SummaryData!B3</f>
+        <v>12</v>
+      </c>
+      <c r="B4" s="10">
+        <f>SummaryData!B4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="10">
-        <f>SummaryData!B4</f>
+        <v>11</v>
+      </c>
+      <c r="B5" s="11">
+        <f>SummaryData!B5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="11">
-        <f>SummaryData!B5</f>
+        <f>SummaryData!B6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="11">
-        <f>SummaryData!B6</f>
+        <v>14</v>
+      </c>
+      <c r="B7" s="10">
+        <f>SummaryData!B7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B8" s="10">
-        <f>SummaryData!B7</f>
+        <f>SummaryData!B8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="10">
-        <f>SummaryData!B8</f>
+        <f>SummaryData!B9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10">
-        <f>SummaryData!B9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1610,7 +1785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37121,19 +37296,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -37142,10 +37316,73 @@
       </c>
       <c r="C1" t="s">
         <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <f>SUM(C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <f>MAX(C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="e">
+        <f>AVERAGE(C:C)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="e">
+        <f>_xlfn.STDEV.P(C:C)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="e">
+        <f>AVEDEV(C:C)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="e">
+        <f>MEDIAN(C:C)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="e">
+        <f>_xlfn.MODE.SNGL(C:C)</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added UTC to rundate column
</commit_message>
<xml_diff>
--- a/Triage/Triage.Mortician.Analyzers/template.xlsx
+++ b/Triage/Triage.Mortician.Analyzers/template.xlsx
@@ -53,9 +53,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>RunDate</t>
-  </si>
-  <si>
     <t>Dump File</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   <si>
     <t>Mode</t>
   </si>
+  <si>
+    <t>RunDate Utc</t>
+  </si>
 </sst>
 </file>
 
@@ -117,11 +117,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -166,43 +173,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,11 +394,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="210880768"/>
-        <c:axId val="211222528"/>
+        <c:axId val="164896128"/>
+        <c:axId val="164906112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210880768"/>
+        <c:axId val="164896128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211222528"/>
+        <c:crossAx val="164906112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -406,7 +416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211222528"/>
+        <c:axId val="164906112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -417,14 +427,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210880768"/>
+        <c:crossAx val="164896128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -605,11 +614,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="210673024"/>
-        <c:axId val="210699392"/>
+        <c:axId val="164932608"/>
+        <c:axId val="164954880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210673024"/>
+        <c:axId val="164932608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210699392"/>
+        <c:crossAx val="164954880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -627,7 +636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210699392"/>
+        <c:axId val="164954880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210673024"/>
+        <c:crossAx val="164932608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -826,11 +835,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="210765312"/>
-        <c:axId val="210766848"/>
+        <c:axId val="164989952"/>
+        <c:axId val="164995840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210765312"/>
+        <c:axId val="164989952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210766848"/>
+        <c:crossAx val="164995840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -848,7 +857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210766848"/>
+        <c:axId val="164995840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,14 +868,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210765312"/>
+        <c:crossAx val="164989952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1047,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="210973440"/>
-        <c:axId val="210974976"/>
+        <c:axId val="166533760"/>
+        <c:axId val="166547840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210973440"/>
+        <c:axId val="166533760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210974976"/>
+        <c:crossAx val="166547840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1069,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210974976"/>
+        <c:axId val="166547840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210973440"/>
+        <c:crossAx val="166533760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1116,7 +1124,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1169,11 +1176,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="226637696"/>
-        <c:axId val="226660352"/>
+        <c:axId val="166557568"/>
+        <c:axId val="166559104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="226637696"/>
+        <c:axId val="166557568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1183,7 +1190,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226660352"/>
+        <c:crossAx val="166559104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1191,7 +1198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="226660352"/>
+        <c:axId val="166559104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,14 +1209,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226637696"/>
+        <c:crossAx val="166557568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1692,7 +1698,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="7">
         <f>SummaryData!B1</f>
@@ -1700,8 +1706,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
+      <c r="A2" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="9">
         <f>SummaryData!B2</f>
@@ -1710,7 +1716,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9">
         <f>SummaryData!B3</f>
@@ -1719,7 +1725,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="10">
         <f>SummaryData!B4</f>
@@ -1728,7 +1734,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="11">
         <f>SummaryData!B5</f>
@@ -1737,7 +1743,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="11">
         <f>SummaryData!B6</f>
@@ -1746,7 +1752,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="10">
         <f>SummaryData!B7</f>
@@ -1755,7 +1761,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="10">
         <f>SummaryData!B8</f>
@@ -1764,7 +1770,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="10">
         <f>SummaryData!B9</f>
@@ -1795,54 +1801,54 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4"/>
     </row>
@@ -37327,7 +37333,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <f>MAX(C:C)</f>
@@ -37336,7 +37342,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" t="e">
         <f>AVERAGE(C:C)</f>
@@ -37345,7 +37351,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="e">
         <f>_xlfn.STDEV.P(C:C)</f>
@@ -37354,7 +37360,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="e">
         <f>AVEDEV(C:C)</f>
@@ -37363,7 +37369,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="e">
         <f>MEDIAN(C:C)</f>
@@ -37372,7 +37378,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="e">
         <f>_xlfn.MODE.SNGL(C:C)</f>

</xml_diff>

<commit_message>
Changed stack grouping to use managed stacks now and not ee stacks
</commit_message>
<xml_diff>
--- a/Triage/Triage.Mortician.Analyzers/template.xlsx
+++ b/Triage/Triage.Mortician.Analyzers/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -394,11 +394,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="164896128"/>
-        <c:axId val="164906112"/>
+        <c:axId val="225779072"/>
+        <c:axId val="225793152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164896128"/>
+        <c:axId val="225779072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164906112"/>
+        <c:crossAx val="225793152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -416,7 +416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164906112"/>
+        <c:axId val="225793152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,7 +427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164896128"/>
+        <c:crossAx val="225779072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -614,11 +614,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="164932608"/>
-        <c:axId val="164954880"/>
+        <c:axId val="225819648"/>
+        <c:axId val="225837824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164932608"/>
+        <c:axId val="225819648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164954880"/>
+        <c:crossAx val="225837824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -636,7 +636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164954880"/>
+        <c:axId val="225837824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164932608"/>
+        <c:crossAx val="225819648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -835,11 +835,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="164989952"/>
-        <c:axId val="164995840"/>
+        <c:axId val="225872896"/>
+        <c:axId val="225878784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164989952"/>
+        <c:axId val="225872896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164995840"/>
+        <c:crossAx val="225878784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -857,7 +857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164995840"/>
+        <c:axId val="225878784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164989952"/>
+        <c:crossAx val="225872896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1055,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="166533760"/>
-        <c:axId val="166547840"/>
+        <c:axId val="226368128"/>
+        <c:axId val="226382208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166533760"/>
+        <c:axId val="226368128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166547840"/>
+        <c:crossAx val="226382208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166547840"/>
+        <c:axId val="226382208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166533760"/>
+        <c:crossAx val="226368128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1124,6 +1124,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1176,11 +1177,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="166557568"/>
-        <c:axId val="166559104"/>
+        <c:axId val="226391936"/>
+        <c:axId val="226393472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166557568"/>
+        <c:axId val="226391936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1191,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166559104"/>
+        <c:crossAx val="226393472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1198,7 +1199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166559104"/>
+        <c:axId val="226393472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,13 +1210,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166557568"/>
+        <c:crossAx val="226391936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1688,7 +1690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37304,7 +37306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37386,7 +37388,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
+  <autoFilter ref="A1:C1">
+    <sortState ref="A2:C3">
+      <sortCondition descending="1" ref="C1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Added some styling to thread excel sheets
</commit_message>
<xml_diff>
--- a/Triage/Triage.Mortician.Analyzers/template.xlsx
+++ b/Triage/Triage.Mortician.Analyzers/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210" activeTab="5"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -217,7 +217,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -394,11 +423,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="225779072"/>
-        <c:axId val="225793152"/>
+        <c:axId val="252394880"/>
+        <c:axId val="252404864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="225779072"/>
+        <c:axId val="252394880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225793152"/>
+        <c:crossAx val="252404864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -416,7 +445,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225793152"/>
+        <c:axId val="252404864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,13 +456,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225779072"/>
+        <c:crossAx val="252394880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -614,11 +644,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="225819648"/>
-        <c:axId val="225837824"/>
+        <c:axId val="252427264"/>
+        <c:axId val="252117760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="225819648"/>
+        <c:axId val="252427264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225837824"/>
+        <c:crossAx val="252117760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -636,7 +666,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225837824"/>
+        <c:axId val="252117760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225819648"/>
+        <c:crossAx val="252427264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -835,11 +865,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="225872896"/>
-        <c:axId val="225878784"/>
+        <c:axId val="252156928"/>
+        <c:axId val="252162816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="225872896"/>
+        <c:axId val="252156928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +879,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225878784"/>
+        <c:crossAx val="252162816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -857,7 +887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225878784"/>
+        <c:axId val="252162816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,13 +898,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225872896"/>
+        <c:crossAx val="252156928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1055,11 +1086,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="226368128"/>
-        <c:axId val="226382208"/>
+        <c:axId val="252328576"/>
+        <c:axId val="252342656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="226368128"/>
+        <c:axId val="252328576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226382208"/>
+        <c:crossAx val="252342656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1108,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="226382208"/>
+        <c:axId val="252342656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1119,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226368128"/>
+        <c:crossAx val="252328576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1177,11 +1208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="226391936"/>
-        <c:axId val="226393472"/>
+        <c:axId val="252542976"/>
+        <c:axId val="252544512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="226391936"/>
+        <c:axId val="252542976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,7 +1222,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226393472"/>
+        <c:crossAx val="252544512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1199,7 +1230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="226393472"/>
+        <c:axId val="252544512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1241,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226391936"/>
+        <c:crossAx val="252542976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1690,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37298,6 +37329,14 @@
     <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="System.">
+      <formula>LEFT(A1,LEN("System."))="System."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="Microsoft.">
+      <formula>LEFT(A1,LEN("Microsoft."))="Microsoft."</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -37306,7 +37345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37393,6 +37432,14 @@
       <sortCondition descending="1" ref="C1"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="System.">
+      <formula>LEFT(A1,LEN("System."))="System."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="Microsoft.">
+      <formula>LEFT(A1,LEN("Microsoft."))="Microsoft."</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>